<commit_message>
update màn hình tạo quảng cáo
</commit_message>
<xml_diff>
--- a/References/Templates/Web MockUp/Prototype Web.xlsx
+++ b/References/Templates/Web MockUp/Prototype Web.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ecchi\Pictures\Web MockUp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Capstone Project\References\Templates\Web MockUp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Danh sách lái xe Dialog" sheetId="3" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="Xóa lái xe" sheetId="2" r:id="rId3"/>
     <sheet name="Cập nhật thông tin lái xe" sheetId="4" r:id="rId4"/>
     <sheet name="Thông tin doanh nghiệp" sheetId="5" r:id="rId5"/>
+    <sheet name="Tạo Quảng Cáo" sheetId="6" r:id="rId6"/>
+    <sheet name="Tạo thông tin khuyến mãi" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
     <t>Số CMND</t>
   </si>
@@ -232,6 +234,27 @@
   </si>
   <si>
     <t>cần phải bổ sung nhiều thông tin liên quan đến doanh nghiệp</t>
+  </si>
+  <si>
+    <t>HOME/Service/Tạo quảng cáo</t>
+  </si>
+  <si>
+    <t>Tên quảng cáo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thời lượng </t>
+  </si>
+  <si>
+    <t>Ảnh</t>
+  </si>
+  <si>
+    <t>Tải ẢNH</t>
+  </si>
+  <si>
+    <t>Đăng quảng cáo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ghi chú (*) : về giá trị và thời lượng quảng cáo . Giá tiền  :                                               </t>
   </si>
 </sst>
 </file>
@@ -611,16 +634,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -631,47 +651,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -684,16 +668,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -705,7 +694,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -718,21 +712,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -745,6 +769,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,25 +1063,25 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="32" t="s">
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -1069,16 +1097,16 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="5"/>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="48"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="44"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -1089,19 +1117,19 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="50"/>
       <c r="I4" s="5"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="48"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="44"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -1112,8 +1140,8 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="45"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="52"/>
       <c r="I5" s="5"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
@@ -1133,8 +1161,8 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="45"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="52"/>
       <c r="I6" s="5"/>
       <c r="K6" s="3"/>
       <c r="L6" s="4"/>
@@ -1154,8 +1182,8 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="55"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="54"/>
       <c r="I7" s="5"/>
       <c r="K7" s="3"/>
       <c r="L7" s="4"/>
@@ -1195,11 +1223,11 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
       <c r="I9" s="5"/>
       <c r="K9" s="3"/>
       <c r="L9" s="4"/>
@@ -1218,11 +1246,11 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
       <c r="I10" s="5"/>
       <c r="K10" s="3"/>
       <c r="L10" s="4"/>
@@ -1241,11 +1269,11 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
       <c r="I11" s="5"/>
       <c r="K11" s="3"/>
       <c r="L11" s="4"/>
@@ -1363,10 +1391,10 @@
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="17"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -1381,15 +1409,15 @@
       <c r="R17" s="5"/>
     </row>
     <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="9"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8"/>
       <c r="K18" s="3"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -1450,25 +1478,25 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="9"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K3:R4"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="G4:H7"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="F11:H11"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K3:R4"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1489,22 +1517,22 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="2"/>
@@ -1517,7 +1545,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="19"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="5"/>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
@@ -1528,38 +1556,38 @@
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="16" t="s">
         <v>28</v>
       </c>
       <c r="I4" s="5"/>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="14"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="21"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="5"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
@@ -1570,101 +1598,101 @@
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="46"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
       <c r="O6" s="4"/>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="14"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
       <c r="O7" s="4"/>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="14"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
       <c r="O8" s="4"/>
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="14"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="5"/>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="14"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="5"/>
@@ -1677,15 +1705,15 @@
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="46"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="5"/>
@@ -1698,13 +1726,13 @@
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="14"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
@@ -1717,13 +1745,13 @@
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="14"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
@@ -1736,13 +1764,13 @@
     </row>
     <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="14"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="5"/>
@@ -1755,13 +1783,13 @@
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="14"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="5"/>
@@ -1774,15 +1802,15 @@
     </row>
     <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="30" t="s">
         <v>51</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="46"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="5"/>
@@ -1830,11 +1858,11 @@
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="14" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="4"/>
@@ -1866,15 +1894,15 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="9"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="8"/>
       <c r="K21" s="3"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -1899,12 +1927,12 @@
       <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="9"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1936,23 +1964,23 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
-      <c r="K2" s="22" t="s">
+      <c r="K2" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -1979,24 +2007,24 @@
     </row>
     <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="14"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="13"/>
       <c r="H4" s="4"/>
       <c r="I4" s="5"/>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="55"/>
+      <c r="P4" s="55"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="5"/>
     </row>
@@ -2010,37 +2038,37 @@
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="5"/>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="48"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="44"/>
     </row>
     <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="17"/>
+      <c r="E6" s="46"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="48"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="44"/>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -2052,63 +2080,63 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="5"/>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="49"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="29"/>
     </row>
     <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="24" t="s">
         <v>40</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="49"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="29"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
-      <c r="B9" s="38">
+      <c r="B9" s="25">
         <v>1</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="39" t="s">
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="26" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="5"/>
@@ -2123,17 +2151,17 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="40">
+      <c r="B10" s="27">
         <v>2</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="41" t="s">
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="28" t="s">
         <v>41</v>
       </c>
       <c r="I10" s="5"/>
@@ -2148,17 +2176,17 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="40">
+      <c r="B11" s="27">
         <v>3</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="41" t="s">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="28" t="s">
         <v>41</v>
       </c>
       <c r="I11" s="5"/>
@@ -2173,17 +2201,17 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
-      <c r="B12" s="40">
+      <c r="B12" s="27">
         <v>4</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="41" t="s">
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="28" t="s">
         <v>41</v>
       </c>
       <c r="I12" s="5"/>
@@ -2198,17 +2226,17 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
-      <c r="B13" s="40">
+      <c r="B13" s="27">
         <v>5</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="41" t="s">
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="28" t="s">
         <v>41</v>
       </c>
       <c r="I13" s="5"/>
@@ -2223,15 +2251,15 @@
     </row>
     <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="42" t="s">
+      <c r="B14" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
       <c r="I14" s="5"/>
       <c r="K14" s="3"/>
       <c r="L14" s="4"/>
@@ -2357,23 +2385,23 @@
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="9"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="9"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="8"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2405,22 +2433,22 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="2"/>
-      <c r="K2" s="24" t="s">
+      <c r="K2" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="2"/>
@@ -2433,7 +2461,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="19"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="5"/>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
@@ -2444,38 +2472,38 @@
     </row>
     <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="16" t="s">
         <v>48</v>
       </c>
       <c r="I4" s="5"/>
-      <c r="K4" s="28" t="s">
+      <c r="K4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="14"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="21"/>
+      <c r="H5" s="17"/>
       <c r="I5" s="5"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
@@ -2486,99 +2514,99 @@
     </row>
     <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="46"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
       <c r="O6" s="4"/>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="14"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="5"/>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
       <c r="O7" s="4"/>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="14"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="55"/>
       <c r="O8" s="4"/>
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="14"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="5"/>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="14"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="5"/>
@@ -2591,15 +2619,15 @@
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="46"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="5"/>
@@ -2612,13 +2640,13 @@
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="14"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="5"/>
@@ -2631,13 +2659,13 @@
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="14"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
@@ -2650,13 +2678,13 @@
     </row>
     <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="14"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="5"/>
@@ -2669,13 +2697,13 @@
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="14"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="5"/>
@@ -2688,15 +2716,15 @@
     </row>
     <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="30" t="s">
         <v>51</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="46"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="5"/>
@@ -2744,11 +2772,11 @@
     <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -2778,15 +2806,15 @@
       <c r="P20" s="5"/>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="9"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="8"/>
       <c r="K21" s="3"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -2811,12 +2839,12 @@
       <c r="P23" s="5"/>
     </row>
     <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="9"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2838,45 +2866,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="58"/>
-      <c r="K2" s="22" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
+      <c r="K2" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="49"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="29"/>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -2886,37 +2914,37 @@
       <c r="Q3" s="5"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="49"/>
-      <c r="K4" s="28" t="s">
+      <c r="A4" s="18"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="29"/>
+      <c r="K4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="49"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="29"/>
     </row>
     <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="49"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="29"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -2926,17 +2954,17 @@
       <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="49"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="29"/>
       <c r="K6" s="3"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -2946,17 +2974,17 @@
       <c r="Q6" s="5"/>
     </row>
     <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="49"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="29"/>
       <c r="K7" s="3"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -2966,17 +2994,17 @@
       <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="49"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="29"/>
       <c r="K8" s="3"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -2986,17 +3014,17 @@
       <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="49"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="29"/>
       <c r="K9" s="3"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -3006,21 +3034,21 @@
       <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="55"/>
+      <c r="C10" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="15" t="s">
+      <c r="D10" s="60"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="49"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="29"/>
       <c r="K10" s="3"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -3030,15 +3058,15 @@
       <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="49"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="29"/>
       <c r="K11" s="3"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -3048,15 +3076,15 @@
       <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="49"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="29"/>
       <c r="K12" s="3"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
@@ -3066,15 +3094,15 @@
       <c r="Q12" s="5"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="49"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="29"/>
       <c r="K13" s="3"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
@@ -3084,15 +3112,15 @@
       <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="28"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="49"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="29"/>
       <c r="K14" s="3"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
@@ -3102,15 +3130,15 @@
       <c r="Q14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="49"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="29"/>
       <c r="K15" s="3"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
@@ -3120,15 +3148,15 @@
       <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="28"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="49"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="29"/>
       <c r="K16" s="3"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
@@ -3138,15 +3166,15 @@
       <c r="Q16" s="5"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="28"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="49"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="29"/>
       <c r="K17" s="3"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
@@ -3156,15 +3184,15 @@
       <c r="Q17" s="5"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="28"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="49"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="29"/>
       <c r="K18" s="3"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
@@ -3174,15 +3202,15 @@
       <c r="Q18" s="5"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="28"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="49"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="29"/>
       <c r="K19" s="3"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
@@ -3192,15 +3220,15 @@
       <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="28"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="49"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="29"/>
       <c r="K20" s="3"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
@@ -3210,15 +3238,15 @@
       <c r="Q20" s="5"/>
     </row>
     <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="59"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="61"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="35"/>
       <c r="K21" s="3"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
@@ -3246,13 +3274,13 @@
       <c r="Q23" s="5"/>
     </row>
     <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="9"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3273,4 +3301,501 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="55"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="46"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B10:H15"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="71"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>